<commit_message>
Added initial Ri3d RoboRIO LabVIEW code to drive 4 motors. Documentation was updated in 2016 Ri3D\Electrical/2016 Ri3d RoboRIO Pinout.xlsx.
</commit_message>
<xml_diff>
--- a/2016/2016 Ri3d/Electrical/2016 Ri3d RoboRIO Pinout.xlsx
+++ b/2016/2016 Ri3d/Electrical/2016 Ri3d RoboRIO Pinout.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>DIO</t>
   </si>
@@ -38,6 +38,21 @@
   </si>
   <si>
     <t>Function</t>
+  </si>
+  <si>
+    <t>Left Rear</t>
+  </si>
+  <si>
+    <t>Left Front</t>
+  </si>
+  <si>
+    <t>Right Rear</t>
+  </si>
+  <si>
+    <t>Right Front</t>
+  </si>
+  <si>
+    <t>SPARK</t>
   </si>
 </sst>
 </file>
@@ -439,15 +454,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B41"/>
+  <dimension ref="A2:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -455,57 +470,57 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -513,57 +528,81 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -571,27 +610,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Tested shooter and beater bar functionality. Moving on to autonomous.
</commit_message>
<xml_diff>
--- a/2016/2016 Ri3d/Electrical/2016 Ri3d RoboRIO Pinout.xlsx
+++ b/2016/2016 Ri3d/Electrical/2016 Ri3d RoboRIO Pinout.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>DIO</t>
   </si>
@@ -53,6 +53,24 @@
   </si>
   <si>
     <t>SPARK</t>
+  </si>
+  <si>
+    <t>Kicker</t>
+  </si>
+  <si>
+    <t>Victor SP</t>
+  </si>
+  <si>
+    <t>Beater Bar</t>
+  </si>
+  <si>
+    <t>Kicker Ready Limit</t>
+  </si>
+  <si>
+    <t>Gyro</t>
+  </si>
+  <si>
+    <t>Gyro Temp</t>
   </si>
 </sst>
 </file>
@@ -457,7 +475,7 @@
   <dimension ref="A2:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,6 +492,9 @@
       <c r="A3">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -576,11 +597,23 @@
       <c r="A19">
         <v>4</v>
       </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -642,10 +675,16 @@
       <c r="A33">
         <v>0</v>
       </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added compressor and solenoid to project.
</commit_message>
<xml_diff>
--- a/2016/2016 Ri3d/Electrical/2016 Ri3d RoboRIO Pinout.xlsx
+++ b/2016/2016 Ri3d/Electrical/2016 Ri3d RoboRIO Pinout.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>DIO</t>
   </si>
@@ -71,6 +71,21 @@
   </si>
   <si>
     <t>Gyro Temp</t>
+  </si>
+  <si>
+    <t>PCM</t>
+  </si>
+  <si>
+    <t>Compressor</t>
+  </si>
+  <si>
+    <t>Pressure Switch</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Intake Lift</t>
   </si>
 </sst>
 </file>
@@ -472,76 +487,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C41"/>
+  <dimension ref="A2:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -549,7 +609,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0</v>
       </c>
@@ -560,7 +620,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Ri3d - 3rd night push. Everything seems to work.
</commit_message>
<xml_diff>
--- a/2016/2016 Ri3d/Electrical/2016 Ri3d RoboRIO Pinout.xlsx
+++ b/2016/2016 Ri3d/Electrical/2016 Ri3d RoboRIO Pinout.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>DIO</t>
   </si>
@@ -40,21 +40,6 @@
     <t>Function</t>
   </si>
   <si>
-    <t>Left Rear</t>
-  </si>
-  <si>
-    <t>Left Front</t>
-  </si>
-  <si>
-    <t>Right Rear</t>
-  </si>
-  <si>
-    <t>Right Front</t>
-  </si>
-  <si>
-    <t>SPARK</t>
-  </si>
-  <si>
     <t>Kicker</t>
   </si>
   <si>
@@ -86,6 +71,15 @@
   </si>
   <si>
     <t>Intake Lift</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>SPARKs</t>
+  </si>
+  <si>
+    <t>Left</t>
   </si>
 </sst>
 </file>
@@ -489,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="161" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,21 +500,18 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -584,21 +575,24 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -614,10 +608,10 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -625,10 +619,10 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
         <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -636,10 +630,10 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -647,33 +641,21 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
@@ -736,7 +718,7 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -744,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added arm code. Plug a Victor SP into PWM5. Use left joystick buttons 6 & 7 to control it.
</commit_message>
<xml_diff>
--- a/2016/2016 Ri3d/Electrical/2016 Ri3d RoboRIO Pinout.xlsx
+++ b/2016/2016 Ri3d/Electrical/2016 Ri3d RoboRIO Pinout.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>DIO</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Left</t>
+  </si>
+  <si>
+    <t>Arm</t>
   </si>
 </sst>
 </file>
@@ -483,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="161" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="161" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,6 +654,12 @@
       <c r="A19">
         <v>4</v>
       </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">

</xml_diff>